<commit_message>
finshed getting flow data
</commit_message>
<xml_diff>
--- a/basin_flow_data.xlsx
+++ b/basin_flow_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Oct</t>
   </si>
@@ -84,6 +84,48 @@
   </si>
   <si>
     <t>mean annual</t>
+  </si>
+  <si>
+    <t>11-norm</t>
+  </si>
+  <si>
+    <t>11-drought</t>
+  </si>
+  <si>
+    <t>12-norm</t>
+  </si>
+  <si>
+    <t>12-drought</t>
+  </si>
+  <si>
+    <t>13-norm</t>
+  </si>
+  <si>
+    <t>13-drought</t>
+  </si>
+  <si>
+    <t>victoria-norm</t>
+  </si>
+  <si>
+    <t>victoria-drought</t>
+  </si>
+  <si>
+    <t>6-norm</t>
+  </si>
+  <si>
+    <t>6-drought</t>
+  </si>
+  <si>
+    <t>kariba-norm</t>
+  </si>
+  <si>
+    <t>kariba-drought</t>
+  </si>
+  <si>
+    <t>Victoria percent</t>
+  </si>
+  <si>
+    <t>kariba percent</t>
   </si>
 </sst>
 </file>
@@ -435,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -465,8 +507,44 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -482,8 +560,54 @@
       <c r="E2">
         <v>266.60000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>13.5</v>
+      </c>
+      <c r="G2">
+        <v>11.4</v>
+      </c>
+      <c r="H2">
+        <v>22.1</v>
+      </c>
+      <c r="I2">
+        <v>18.7</v>
+      </c>
+      <c r="J2">
+        <v>79.5</v>
+      </c>
+      <c r="K2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="L2">
+        <v>82</v>
+      </c>
+      <c r="M2">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="N2">
+        <v>386.7</v>
+      </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <f>N2*0.1</f>
+        <v>38.67</v>
+      </c>
+      <c r="Q2">
+        <f>O2*0.1</f>
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <f>N2*0.9</f>
+        <v>348.03</v>
+      </c>
+      <c r="S2">
+        <f>O2*0.9</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -499,8 +623,54 @@
       <c r="E3">
         <v>259.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>13.3</v>
+      </c>
+      <c r="G3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H3">
+        <v>21.9</v>
+      </c>
+      <c r="I3">
+        <v>15.3</v>
+      </c>
+      <c r="J3">
+        <v>110.5</v>
+      </c>
+      <c r="K3">
+        <v>43.3</v>
+      </c>
+      <c r="L3">
+        <v>102.8</v>
+      </c>
+      <c r="M3">
+        <v>80.5</v>
+      </c>
+      <c r="N3">
+        <v>402.3</v>
+      </c>
+      <c r="O3">
+        <v>292.60000000000002</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P14" si="0">N3*0.1</f>
+        <v>40.230000000000004</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q14" si="1">O3*0.1</f>
+        <v>29.260000000000005</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R14" si="2">N3*0.9</f>
+        <v>362.07</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S14" si="3">O3*0.9</f>
+        <v>263.34000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -516,8 +686,54 @@
       <c r="E4">
         <v>275.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>18.3</v>
+      </c>
+      <c r="G4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H4">
+        <v>29.9</v>
+      </c>
+      <c r="I4">
+        <v>15.3</v>
+      </c>
+      <c r="J4">
+        <v>274.60000000000002</v>
+      </c>
+      <c r="K4">
+        <v>80.5</v>
+      </c>
+      <c r="L4">
+        <v>203.3</v>
+      </c>
+      <c r="M4">
+        <v>104.2</v>
+      </c>
+      <c r="N4">
+        <v>817.4</v>
+      </c>
+      <c r="O4">
+        <v>215.2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>81.740000000000009</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>21.52</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>735.66</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>193.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -533,8 +749,54 @@
       <c r="E5">
         <v>389.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>52</v>
+      </c>
+      <c r="G5">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H5">
+        <v>85.2</v>
+      </c>
+      <c r="I5">
+        <v>16.3</v>
+      </c>
+      <c r="J5">
+        <v>795.3</v>
+      </c>
+      <c r="K5">
+        <v>157.5</v>
+      </c>
+      <c r="L5">
+        <v>354.5</v>
+      </c>
+      <c r="M5">
+        <v>190.6</v>
+      </c>
+      <c r="N5">
+        <v>1265.3</v>
+      </c>
+      <c r="O5">
+        <v>327.10000000000002</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>126.53</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>32.71</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>1138.77</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>294.39000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -550,8 +812,54 @@
       <c r="E6">
         <v>500.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>119.6</v>
+      </c>
+      <c r="G6">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H6">
+        <v>196.1</v>
+      </c>
+      <c r="I6">
+        <v>15.3</v>
+      </c>
+      <c r="J6">
+        <v>1674</v>
+      </c>
+      <c r="K6">
+        <v>310.10000000000002</v>
+      </c>
+      <c r="L6">
+        <v>532.9</v>
+      </c>
+      <c r="M6">
+        <v>204.8</v>
+      </c>
+      <c r="N6">
+        <v>2073.1999999999998</v>
+      </c>
+      <c r="O6">
+        <v>464</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>207.32</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>46.400000000000006</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>1865.8799999999999</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>417.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -567,8 +875,54 @@
       <c r="E7">
         <v>730.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>227.7</v>
+      </c>
+      <c r="G7">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H7">
+        <v>373.4</v>
+      </c>
+      <c r="I7">
+        <v>28.9</v>
+      </c>
+      <c r="J7">
+        <v>2304.1</v>
+      </c>
+      <c r="K7">
+        <v>873.9</v>
+      </c>
+      <c r="L7">
+        <v>664.6</v>
+      </c>
+      <c r="M7">
+        <v>339.8</v>
+      </c>
+      <c r="N7">
+        <v>2485.3000000000002</v>
+      </c>
+      <c r="O7">
+        <v>725.2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>248.53000000000003</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>72.52000000000001</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>2236.7700000000004</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>652.68000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -584,8 +938,54 @@
       <c r="E8">
         <v>1047.9000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>181.6</v>
+      </c>
+      <c r="G8">
+        <v>30.1</v>
+      </c>
+      <c r="H8">
+        <v>297.7</v>
+      </c>
+      <c r="I8">
+        <v>49.3</v>
+      </c>
+      <c r="J8">
+        <v>2037</v>
+      </c>
+      <c r="K8">
+        <v>758.5</v>
+      </c>
+      <c r="L8">
+        <v>558.4</v>
+      </c>
+      <c r="M8">
+        <v>230.9</v>
+      </c>
+      <c r="N8">
+        <v>2927.6</v>
+      </c>
+      <c r="O8">
+        <v>1369.8</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>292.76</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>136.97999999999999</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>2634.84</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>1232.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -601,8 +1001,54 @@
       <c r="E9">
         <v>1018</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>88.7</v>
+      </c>
+      <c r="G9">
+        <v>22.8</v>
+      </c>
+      <c r="H9">
+        <v>145.5</v>
+      </c>
+      <c r="I9">
+        <v>37.4</v>
+      </c>
+      <c r="J9">
+        <v>799.3</v>
+      </c>
+      <c r="K9">
+        <v>333</v>
+      </c>
+      <c r="L9">
+        <v>270</v>
+      </c>
+      <c r="M9">
+        <v>125.59</v>
+      </c>
+      <c r="N9">
+        <v>2612.4</v>
+      </c>
+      <c r="O9">
+        <v>1224.3</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>261.24</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>122.43</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>2351.1600000000003</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>1101.8699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -618,8 +1064,54 @@
       <c r="E10">
         <v>480.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>49</v>
+      </c>
+      <c r="G10">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H10">
+        <v>80.3</v>
+      </c>
+      <c r="I10">
+        <v>28.9</v>
+      </c>
+      <c r="J10">
+        <v>366.2</v>
+      </c>
+      <c r="K10">
+        <v>180.3</v>
+      </c>
+      <c r="L10">
+        <v>166.7</v>
+      </c>
+      <c r="M10">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>1657.4</v>
+      </c>
+      <c r="O10">
+        <v>473.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>165.74</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>47.35</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>1491.66</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>426.15000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -635,8 +1127,54 @@
       <c r="E11">
         <v>333.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>30.8</v>
+      </c>
+      <c r="G11">
+        <v>15.6</v>
+      </c>
+      <c r="H11">
+        <v>50.5</v>
+      </c>
+      <c r="I11">
+        <v>25.5</v>
+      </c>
+      <c r="J11">
+        <v>221.6</v>
+      </c>
+      <c r="K11">
+        <v>113</v>
+      </c>
+      <c r="L11">
+        <v>137.30000000000001</v>
+      </c>
+      <c r="M11">
+        <v>80.5</v>
+      </c>
+      <c r="N11">
+        <v>910.1</v>
+      </c>
+      <c r="O11">
+        <v>296.39999999999998</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>91.01</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>29.64</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>819.09</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>266.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -652,8 +1190,54 @@
       <c r="E12">
         <v>274.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>21.9</v>
+      </c>
+      <c r="G12">
+        <v>12.4</v>
+      </c>
+      <c r="H12">
+        <v>35.9</v>
+      </c>
+      <c r="I12">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>144</v>
+      </c>
+      <c r="K12">
+        <v>80.5</v>
+      </c>
+      <c r="L12">
+        <v>113.8</v>
+      </c>
+      <c r="M12">
+        <v>72.2</v>
+      </c>
+      <c r="N12">
+        <v>605</v>
+      </c>
+      <c r="O12">
+        <v>344.6</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>60.5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>34.46</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>544.5</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>310.14000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -669,8 +1253,54 @@
       <c r="E13">
         <v>237.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>16.2</v>
+      </c>
+      <c r="G13">
+        <v>10.4</v>
+      </c>
+      <c r="H13">
+        <v>26.6</v>
+      </c>
+      <c r="I13">
+        <v>17</v>
+      </c>
+      <c r="J13">
+        <v>96.3</v>
+      </c>
+      <c r="K13">
+        <v>55.3</v>
+      </c>
+      <c r="L13">
+        <v>89.8</v>
+      </c>
+      <c r="M13">
+        <v>60.4</v>
+      </c>
+      <c r="N13">
+        <v>490.4</v>
+      </c>
+      <c r="O13">
+        <v>335.1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>49.04</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>33.510000000000005</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>441.36</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>301.59000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -685,6 +1315,66 @@
       </c>
       <c r="E14">
         <v>484.5</v>
+      </c>
+      <c r="F14">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G14">
+        <v>14.6</v>
+      </c>
+      <c r="H14">
+        <v>113.8</v>
+      </c>
+      <c r="I14">
+        <v>23.9</v>
+      </c>
+      <c r="J14">
+        <v>741.9</v>
+      </c>
+      <c r="K14">
+        <v>251.9</v>
+      </c>
+      <c r="L14">
+        <v>273</v>
+      </c>
+      <c r="M14">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="N14">
+        <v>1386.1</v>
+      </c>
+      <c r="O14">
+        <v>522.29999999999995</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>138.60999999999999</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>52.23</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="2"/>
+        <v>1247.49</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>470.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15">
+        <v>0.1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished writing up flow data in basin_flow_dat
</commit_message>
<xml_diff>
--- a/basin_flow_data.xlsx
+++ b/basin_flow_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Oct</t>
   </si>
@@ -84,6 +84,48 @@
   </si>
   <si>
     <t>mean annual</t>
+  </si>
+  <si>
+    <t>11-norm</t>
+  </si>
+  <si>
+    <t>11-drought</t>
+  </si>
+  <si>
+    <t>12-norm</t>
+  </si>
+  <si>
+    <t>12-drought</t>
+  </si>
+  <si>
+    <t>13-norm</t>
+  </si>
+  <si>
+    <t>13-drought</t>
+  </si>
+  <si>
+    <t>victoria-norm</t>
+  </si>
+  <si>
+    <t>victoria-drought</t>
+  </si>
+  <si>
+    <t>6-norm</t>
+  </si>
+  <si>
+    <t>6-drought</t>
+  </si>
+  <si>
+    <t>kariba-norm</t>
+  </si>
+  <si>
+    <t>kariba-drought</t>
+  </si>
+  <si>
+    <t>Victoria percent</t>
+  </si>
+  <si>
+    <t>kariba percent</t>
   </si>
 </sst>
 </file>
@@ -435,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -465,8 +507,44 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -482,8 +560,54 @@
       <c r="E2">
         <v>266.60000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>13.5</v>
+      </c>
+      <c r="G2">
+        <v>11.4</v>
+      </c>
+      <c r="H2">
+        <v>22.1</v>
+      </c>
+      <c r="I2">
+        <v>18.7</v>
+      </c>
+      <c r="J2">
+        <v>79.5</v>
+      </c>
+      <c r="K2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="L2">
+        <v>82</v>
+      </c>
+      <c r="M2">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="N2">
+        <v>386.7</v>
+      </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <f>N2*0.1</f>
+        <v>38.67</v>
+      </c>
+      <c r="Q2">
+        <f>O2*0.1</f>
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <f>N2*0.9</f>
+        <v>348.03</v>
+      </c>
+      <c r="S2">
+        <f>O2*0.9</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -499,8 +623,54 @@
       <c r="E3">
         <v>259.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>13.3</v>
+      </c>
+      <c r="G3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H3">
+        <v>21.9</v>
+      </c>
+      <c r="I3">
+        <v>15.3</v>
+      </c>
+      <c r="J3">
+        <v>110.5</v>
+      </c>
+      <c r="K3">
+        <v>43.3</v>
+      </c>
+      <c r="L3">
+        <v>102.8</v>
+      </c>
+      <c r="M3">
+        <v>80.5</v>
+      </c>
+      <c r="N3">
+        <v>402.3</v>
+      </c>
+      <c r="O3">
+        <v>292.60000000000002</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P14" si="0">N3*0.1</f>
+        <v>40.230000000000004</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q14" si="1">O3*0.1</f>
+        <v>29.260000000000005</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R14" si="2">N3*0.9</f>
+        <v>362.07</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S14" si="3">O3*0.9</f>
+        <v>263.34000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -516,8 +686,54 @@
       <c r="E4">
         <v>275.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>18.3</v>
+      </c>
+      <c r="G4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H4">
+        <v>29.9</v>
+      </c>
+      <c r="I4">
+        <v>15.3</v>
+      </c>
+      <c r="J4">
+        <v>274.60000000000002</v>
+      </c>
+      <c r="K4">
+        <v>80.5</v>
+      </c>
+      <c r="L4">
+        <v>203.3</v>
+      </c>
+      <c r="M4">
+        <v>104.2</v>
+      </c>
+      <c r="N4">
+        <v>817.4</v>
+      </c>
+      <c r="O4">
+        <v>215.2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>81.740000000000009</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>21.52</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>735.66</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>193.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -533,8 +749,54 @@
       <c r="E5">
         <v>389.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>52</v>
+      </c>
+      <c r="G5">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H5">
+        <v>85.2</v>
+      </c>
+      <c r="I5">
+        <v>16.3</v>
+      </c>
+      <c r="J5">
+        <v>795.3</v>
+      </c>
+      <c r="K5">
+        <v>157.5</v>
+      </c>
+      <c r="L5">
+        <v>354.5</v>
+      </c>
+      <c r="M5">
+        <v>190.6</v>
+      </c>
+      <c r="N5">
+        <v>1265.3</v>
+      </c>
+      <c r="O5">
+        <v>327.10000000000002</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>126.53</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>32.71</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>1138.77</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>294.39000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -550,8 +812,54 @@
       <c r="E6">
         <v>500.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>119.6</v>
+      </c>
+      <c r="G6">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H6">
+        <v>196.1</v>
+      </c>
+      <c r="I6">
+        <v>15.3</v>
+      </c>
+      <c r="J6">
+        <v>1674</v>
+      </c>
+      <c r="K6">
+        <v>310.10000000000002</v>
+      </c>
+      <c r="L6">
+        <v>532.9</v>
+      </c>
+      <c r="M6">
+        <v>204.8</v>
+      </c>
+      <c r="N6">
+        <v>2073.1999999999998</v>
+      </c>
+      <c r="O6">
+        <v>464</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>207.32</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>46.400000000000006</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>1865.8799999999999</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>417.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -567,8 +875,54 @@
       <c r="E7">
         <v>730.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>227.7</v>
+      </c>
+      <c r="G7">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H7">
+        <v>373.4</v>
+      </c>
+      <c r="I7">
+        <v>28.9</v>
+      </c>
+      <c r="J7">
+        <v>2304.1</v>
+      </c>
+      <c r="K7">
+        <v>873.9</v>
+      </c>
+      <c r="L7">
+        <v>664.6</v>
+      </c>
+      <c r="M7">
+        <v>339.8</v>
+      </c>
+      <c r="N7">
+        <v>2485.3000000000002</v>
+      </c>
+      <c r="O7">
+        <v>725.2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>248.53000000000003</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>72.52000000000001</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>2236.7700000000004</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>652.68000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -584,8 +938,54 @@
       <c r="E8">
         <v>1047.9000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>181.6</v>
+      </c>
+      <c r="G8">
+        <v>30.1</v>
+      </c>
+      <c r="H8">
+        <v>297.7</v>
+      </c>
+      <c r="I8">
+        <v>49.3</v>
+      </c>
+      <c r="J8">
+        <v>2037</v>
+      </c>
+      <c r="K8">
+        <v>758.5</v>
+      </c>
+      <c r="L8">
+        <v>558.4</v>
+      </c>
+      <c r="M8">
+        <v>230.9</v>
+      </c>
+      <c r="N8">
+        <v>2927.6</v>
+      </c>
+      <c r="O8">
+        <v>1369.8</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>292.76</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>136.97999999999999</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>2634.84</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>1232.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -601,8 +1001,54 @@
       <c r="E9">
         <v>1018</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>88.7</v>
+      </c>
+      <c r="G9">
+        <v>22.8</v>
+      </c>
+      <c r="H9">
+        <v>145.5</v>
+      </c>
+      <c r="I9">
+        <v>37.4</v>
+      </c>
+      <c r="J9">
+        <v>799.3</v>
+      </c>
+      <c r="K9">
+        <v>333</v>
+      </c>
+      <c r="L9">
+        <v>270</v>
+      </c>
+      <c r="M9">
+        <v>125.59</v>
+      </c>
+      <c r="N9">
+        <v>2612.4</v>
+      </c>
+      <c r="O9">
+        <v>1224.3</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>261.24</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>122.43</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>2351.1600000000003</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>1101.8699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -618,8 +1064,54 @@
       <c r="E10">
         <v>480.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>49</v>
+      </c>
+      <c r="G10">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H10">
+        <v>80.3</v>
+      </c>
+      <c r="I10">
+        <v>28.9</v>
+      </c>
+      <c r="J10">
+        <v>366.2</v>
+      </c>
+      <c r="K10">
+        <v>180.3</v>
+      </c>
+      <c r="L10">
+        <v>166.7</v>
+      </c>
+      <c r="M10">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>1657.4</v>
+      </c>
+      <c r="O10">
+        <v>473.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>165.74</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>47.35</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>1491.66</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>426.15000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -635,8 +1127,54 @@
       <c r="E11">
         <v>333.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>30.8</v>
+      </c>
+      <c r="G11">
+        <v>15.6</v>
+      </c>
+      <c r="H11">
+        <v>50.5</v>
+      </c>
+      <c r="I11">
+        <v>25.5</v>
+      </c>
+      <c r="J11">
+        <v>221.6</v>
+      </c>
+      <c r="K11">
+        <v>113</v>
+      </c>
+      <c r="L11">
+        <v>137.30000000000001</v>
+      </c>
+      <c r="M11">
+        <v>80.5</v>
+      </c>
+      <c r="N11">
+        <v>910.1</v>
+      </c>
+      <c r="O11">
+        <v>296.39999999999998</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>91.01</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>29.64</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>819.09</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>266.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -652,8 +1190,54 @@
       <c r="E12">
         <v>274.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>21.9</v>
+      </c>
+      <c r="G12">
+        <v>12.4</v>
+      </c>
+      <c r="H12">
+        <v>35.9</v>
+      </c>
+      <c r="I12">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>144</v>
+      </c>
+      <c r="K12">
+        <v>80.5</v>
+      </c>
+      <c r="L12">
+        <v>113.8</v>
+      </c>
+      <c r="M12">
+        <v>72.2</v>
+      </c>
+      <c r="N12">
+        <v>605</v>
+      </c>
+      <c r="O12">
+        <v>344.6</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>60.5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>34.46</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>544.5</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>310.14000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -669,8 +1253,54 @@
       <c r="E13">
         <v>237.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>16.2</v>
+      </c>
+      <c r="G13">
+        <v>10.4</v>
+      </c>
+      <c r="H13">
+        <v>26.6</v>
+      </c>
+      <c r="I13">
+        <v>17</v>
+      </c>
+      <c r="J13">
+        <v>96.3</v>
+      </c>
+      <c r="K13">
+        <v>55.3</v>
+      </c>
+      <c r="L13">
+        <v>89.8</v>
+      </c>
+      <c r="M13">
+        <v>60.4</v>
+      </c>
+      <c r="N13">
+        <v>490.4</v>
+      </c>
+      <c r="O13">
+        <v>335.1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>49.04</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>33.510000000000005</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>441.36</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>301.59000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -685,6 +1315,66 @@
       </c>
       <c r="E14">
         <v>484.5</v>
+      </c>
+      <c r="F14">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G14">
+        <v>14.6</v>
+      </c>
+      <c r="H14">
+        <v>113.8</v>
+      </c>
+      <c r="I14">
+        <v>23.9</v>
+      </c>
+      <c r="J14">
+        <v>741.9</v>
+      </c>
+      <c r="K14">
+        <v>251.9</v>
+      </c>
+      <c r="L14">
+        <v>273</v>
+      </c>
+      <c r="M14">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="N14">
+        <v>1386.1</v>
+      </c>
+      <c r="O14">
+        <v>522.29999999999995</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>138.60999999999999</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>52.23</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="2"/>
+        <v>1247.49</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>470.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15">
+        <v>0.1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>